<commit_message>
Update Planning, Add mcd
</commit_message>
<xml_diff>
--- a/doc/Planning.xlsx
+++ b/doc/Planning.xlsx
@@ -817,9 +817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:MX33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N28" sqref="N28"/>
+      <selection pane="topRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10738,58 +10738,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="LF1:LJ1"/>
-    <mergeCell ref="LK1:LO1"/>
-    <mergeCell ref="LP1:LT1"/>
-    <mergeCell ref="LU1:LY1"/>
-    <mergeCell ref="LA1:LE1"/>
-    <mergeCell ref="IX1:JB1"/>
-    <mergeCell ref="JC1:JG1"/>
-    <mergeCell ref="JH1:JL1"/>
-    <mergeCell ref="JM1:JQ1"/>
-    <mergeCell ref="JR1:JV1"/>
-    <mergeCell ref="JW1:KA1"/>
-    <mergeCell ref="KB1:KF1"/>
-    <mergeCell ref="KG1:KK1"/>
-    <mergeCell ref="KL1:KP1"/>
-    <mergeCell ref="KQ1:KU1"/>
-    <mergeCell ref="KV1:KZ1"/>
-    <mergeCell ref="IS1:IW1"/>
-    <mergeCell ref="GP1:GT1"/>
-    <mergeCell ref="GU1:GY1"/>
-    <mergeCell ref="GZ1:HD1"/>
-    <mergeCell ref="HE1:HI1"/>
-    <mergeCell ref="HJ1:HN1"/>
-    <mergeCell ref="HO1:HS1"/>
-    <mergeCell ref="HT1:HX1"/>
-    <mergeCell ref="HY1:IC1"/>
-    <mergeCell ref="ID1:IH1"/>
-    <mergeCell ref="II1:IM1"/>
-    <mergeCell ref="IN1:IR1"/>
-    <mergeCell ref="GK1:GO1"/>
-    <mergeCell ref="EH1:EL1"/>
-    <mergeCell ref="EM1:EQ1"/>
-    <mergeCell ref="ER1:EV1"/>
-    <mergeCell ref="EW1:FA1"/>
-    <mergeCell ref="FB1:FF1"/>
-    <mergeCell ref="FG1:FK1"/>
-    <mergeCell ref="FL1:FP1"/>
-    <mergeCell ref="FQ1:FU1"/>
-    <mergeCell ref="FV1:FZ1"/>
-    <mergeCell ref="GA1:GE1"/>
-    <mergeCell ref="GF1:GJ1"/>
-    <mergeCell ref="EC1:EG1"/>
-    <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="CE1:CI1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CO1:CS1"/>
-    <mergeCell ref="CT1:CX1"/>
-    <mergeCell ref="CY1:DC1"/>
-    <mergeCell ref="DD1:DH1"/>
-    <mergeCell ref="DI1:DM1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DS1:DW1"/>
-    <mergeCell ref="DX1:EB1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
@@ -10805,6 +10753,58 @@
     <mergeCell ref="BF1:BJ1"/>
     <mergeCell ref="BK1:BO1"/>
     <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="EC1:EG1"/>
+    <mergeCell ref="BZ1:CD1"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CO1:CS1"/>
+    <mergeCell ref="CT1:CX1"/>
+    <mergeCell ref="CY1:DC1"/>
+    <mergeCell ref="DD1:DH1"/>
+    <mergeCell ref="DI1:DM1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DS1:DW1"/>
+    <mergeCell ref="DX1:EB1"/>
+    <mergeCell ref="GK1:GO1"/>
+    <mergeCell ref="EH1:EL1"/>
+    <mergeCell ref="EM1:EQ1"/>
+    <mergeCell ref="ER1:EV1"/>
+    <mergeCell ref="EW1:FA1"/>
+    <mergeCell ref="FB1:FF1"/>
+    <mergeCell ref="FG1:FK1"/>
+    <mergeCell ref="FL1:FP1"/>
+    <mergeCell ref="FQ1:FU1"/>
+    <mergeCell ref="FV1:FZ1"/>
+    <mergeCell ref="GA1:GE1"/>
+    <mergeCell ref="GF1:GJ1"/>
+    <mergeCell ref="KV1:KZ1"/>
+    <mergeCell ref="IS1:IW1"/>
+    <mergeCell ref="GP1:GT1"/>
+    <mergeCell ref="GU1:GY1"/>
+    <mergeCell ref="GZ1:HD1"/>
+    <mergeCell ref="HE1:HI1"/>
+    <mergeCell ref="HJ1:HN1"/>
+    <mergeCell ref="HO1:HS1"/>
+    <mergeCell ref="HT1:HX1"/>
+    <mergeCell ref="HY1:IC1"/>
+    <mergeCell ref="ID1:IH1"/>
+    <mergeCell ref="II1:IM1"/>
+    <mergeCell ref="IN1:IR1"/>
+    <mergeCell ref="JW1:KA1"/>
+    <mergeCell ref="KB1:KF1"/>
+    <mergeCell ref="KG1:KK1"/>
+    <mergeCell ref="KL1:KP1"/>
+    <mergeCell ref="KQ1:KU1"/>
+    <mergeCell ref="IX1:JB1"/>
+    <mergeCell ref="JC1:JG1"/>
+    <mergeCell ref="JH1:JL1"/>
+    <mergeCell ref="JM1:JQ1"/>
+    <mergeCell ref="JR1:JV1"/>
+    <mergeCell ref="LF1:LJ1"/>
+    <mergeCell ref="LK1:LO1"/>
+    <mergeCell ref="LP1:LT1"/>
+    <mergeCell ref="LU1:LY1"/>
+    <mergeCell ref="LA1:LE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>